<commit_message>
Removed poorly specified tests
 - Renamed parameter name for oneOf
</commit_message>
<xml_diff>
--- a/ExcelToEnumerable.Tests/TestSpreadsheets/MostComplexExample.xlsx
+++ b/ExcelToEnumerable.Tests/TestSpreadsheets/MostComplexExample.xlsx
@@ -347,7 +347,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -371,6 +371,95 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -379,7 +468,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,12 +477,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFCE4D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFCE4D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
         <bgColor rgb="FFC00000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFCC0000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -401,8 +532,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -426,17 +572,68 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -456,15 +653,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -476,23 +673,44 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Status 10" xfId="34"/>
+    <cellStyle name="Text 6" xfId="35"/>
+    <cellStyle name="Warning 14" xfId="36"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
       <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF00B050"/>
+        <sz val="11"/>
       </font>
       <fill>
         <patternFill>
@@ -502,7 +720,11 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FFC00000"/>
+        <sz val="11"/>
       </font>
       <fill>
         <patternFill>
@@ -511,6 +733,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFFF"/>
@@ -525,6 +754,13 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFCE4D6"/>
@@ -532,22 +768,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
-        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
       </font>
       <fill>
         <patternFill>
@@ -557,22 +783,12 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -581,7 +797,11 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF00B050"/>
+        <sz val="11"/>
       </font>
       <fill>
         <patternFill>
@@ -591,7 +811,67 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FFC00000"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF00B050"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFC00000"/>
+        <sz val="11"/>
       </font>
       <fill>
         <patternFill>
@@ -606,42 +886,42 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FFC00000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFCE4D6"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFCE4D6"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -671,14 +951,14 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4:N27"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="16.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.88"/>
@@ -692,8 +972,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="18.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="3" width="18.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="20" style="3" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1017" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="20" style="3" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="152.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1084,9 +1363,7 @@
       <c r="G7" s="2" t="n">
         <v>1.01</v>
       </c>
-      <c r="H7" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1142,7 +1419,7 @@
         <v>1.01</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>29</v>
@@ -1891,7 +2168,7 @@
         <v>29</v>
       </c>
       <c r="J21" s="6" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="K21" s="6" t="n">
         <v>1</v>
@@ -30260,9 +30537,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A3894">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28:I3894 E28:G3894 E3:I27">
     <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
@@ -30292,33 +30567,37 @@
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G3:H1027" type="decimal">
       <formula1>0.00001</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I3:I1027" type="list">
+      <formula1>Keys!$F$5:$F$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J3:K20 K21:K27 J22:J27 J28:K1027" type="whole">
+      <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L3:L1027" type="decimal">
       <formula1>0.01</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J3:K1027" type="whole">
-      <formula1>1</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M3:M1027" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M3:M1027" type="list">
       <formula1>Keys!$I$5:$I$12</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I3:I1027" type="list">
-      <formula1>Keys!$F$5:$F$8</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R3:S26 S27 R28:S1027" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R3:S26 S27 R28:S1027" type="list">
       <formula1>Keys!$V$3:$V$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R27" type="none">
-      <formula1>Keys!$V$3:$V$4</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R27" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J21" type="none">
+      <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -30340,10 +30619,10 @@
   <dimension ref="A2:V13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="1" sqref="B4:N27 R2"/>
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="9.13"/>
@@ -30358,7 +30637,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="12" style="6" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="6" width="11.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30560,7 +30838,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="e62d"/>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -30579,13 +30857,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:N27 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.37"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="n">
@@ -30593,7 +30868,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="e62d"/>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>